<commit_message>
Removes CO2 as a separately regulated pollutant
</commit_message>
<xml_diff>
--- a/InputData/trans/SRPbVT/Separately Regulated Pollutants by Vehicle Type.xlsx
+++ b/InputData/trans/SRPbVT/Separately Regulated Pollutants by Vehicle Type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energyinnovation.sharepoint.com/sites/EUEPSModeling/Shared Documents/InputData_EI+Agora/trans/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\trans\SRPbVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1911C4-ACC9-48DC-8478-29DA285D1462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B633D6B-94A0-4482-8CAB-52E1A4120A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33840" yWindow="-1200" windowWidth="21420" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -628,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
@@ -981,8 +981,8 @@
   </sheetPr>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1036,7 +1036,7 @@
         <v>71</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1077,7 +1077,7 @@
         <v>72</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1118,7 +1118,7 @@
         <v>73</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1283,26 +1283,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -1525,10 +1505,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14F2E2C9-A228-4164-9031-D28FFE5F7873}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17CAF422-1580-4048-9C6D-691986306A53}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1545,20 +1556,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17CAF422-1580-4048-9C6D-691986306A53}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14F2E2C9-A228-4164-9031-D28FFE5F7873}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>